<commit_message>
Update Jupyter Notebook Examples
</commit_message>
<xml_diff>
--- a/data/kiel_arbeitslose.xlsx
+++ b/data/kiel_arbeitslose.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bodo/Documents/dev/Python/Kiel_Open_Data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{442C4E0E-D22A-5D42-8992-EEF8AEFA4F9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -38,8 +39,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -71,6 +72,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -96,22 +104,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -379,11 +391,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:B28"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -616,6 +628,38 @@
         <v>12867</v>
       </c>
     </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>2017</v>
+      </c>
+      <c r="B29" s="2">
+        <v>11939</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>2018</v>
+      </c>
+      <c r="B30" s="2">
+        <v>10260</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>2019</v>
+      </c>
+      <c r="B31" s="2">
+        <v>10009</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>2020</v>
+      </c>
+      <c r="B32" s="2">
+        <v>11776</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>